<commit_message>
updating weights for aggregation
</commit_message>
<xml_diff>
--- a/R_code/model_xwalk.xlsx
+++ b/R_code/model_xwalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nmath_000\Documents\Research\Heterogeneous-Teacher-Value-Added\R_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0516D64-2FD9-4B7E-B9E5-49DDC7B41348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E896E6-9C37-4069-8D5C-F6D752F1A89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{122CD9DC-2F6C-4F1E-8C88-32DFF68959F5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t xml:space="preserve">nsims </t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>linear</t>
+  </si>
+  <si>
+    <t>weight_below</t>
+  </si>
+  <si>
+    <t>weight_above</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2D317C-9CA4-413E-857F-0A2C0E516F71}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -510,12 +516,14 @@
     <col min="8" max="8" width="12.15625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.83984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.41796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.83984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -549,17 +557,23 @@
       <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -590,8 +604,14 @@
       <c r="K2">
         <v>0.4</v>
       </c>
+      <c r="L2">
+        <v>0.2</v>
+      </c>
+      <c r="M2">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -622,8 +642,14 @@
       <c r="K3">
         <v>0.4</v>
       </c>
+      <c r="L3">
+        <v>0.2</v>
+      </c>
+      <c r="M3">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Add one parameter to the model_xwalk
</commit_message>
<xml_diff>
--- a/R_code/model_xwalk.xlsx
+++ b/R_code/model_xwalk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t xml:space="preserve">run_id </t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">npoints</t>
   </si>
   <si>
+    <t xml:space="preserve">single_run</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_teacher</t>
   </si>
   <si>
@@ -58,6 +61,24 @@
     <t xml:space="preserve">method</t>
   </si>
   <si>
+    <t xml:space="preserve">covariates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peer_effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stud_sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ta_sd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sa_sd</t>
+  </si>
+  <si>
     <t xml:space="preserve">lin_alpha</t>
   </si>
   <si>
@@ -86,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qtle</t>
   </si>
 </sst>
 </file>
@@ -304,10 +328,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,22 +339,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="4.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="14" style="0" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="7.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="5.73"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -370,26 +394,47 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,46 +442,67 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>0.05</v>
-      </c>
       <c r="G2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="O2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="R2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V2" s="0" t="n">
         <v>0.8</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,93 +510,67 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="F3" s="0" t="n">
-        <v>0.05</v>
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="O3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="R3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V3" s="0" t="n">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="O4" s="0" t="n">
+      <c r="W3" s="0" t="n">
         <v>0.2</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for full Monte Carlo run
</commit_message>
<xml_diff>
--- a/R_code/model_xwalk.xlsx
+++ b/R_code/model_xwalk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="31">
   <si>
     <t xml:space="preserve">run_id </t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
   </si>
   <si>
     <t xml:space="preserve">qtle</t>
@@ -328,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -442,16 +445,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>30</v>
@@ -469,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>27</v>
@@ -490,10 +493,13 @@
         <v>0.2</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="U2" s="0" t="n">
         <v>0.3</v>
@@ -503,6 +509,15 @@
       </c>
       <c r="W2" s="0" t="n">
         <v>0.2</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1000</v>
@@ -519,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>30</v>
@@ -537,16 +552,16 @@
         <v>1</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L3" s="0" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>0</v>
@@ -558,10 +573,13 @@
         <v>0.2</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S3" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>0.3</v>
@@ -571,6 +589,1135 @@
       </c>
       <c r="W3" s="0" t="n">
         <v>0.2</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V9" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W9" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W11" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z16" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="U17" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="V17" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z17" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>